<commit_message>
Made changes to database build and spreadsheet
</commit_message>
<xml_diff>
--- a/Lesson_04 - Simple Select Queries Pt 2/employees.xlsx
+++ b/Lesson_04 - Simple Select Queries Pt 2/employees.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
   <si>
     <t xml:space="preserve">EMPLOYEE_NAME</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">sarah@email.com</t>
   </si>
   <si>
-    <t xml:space="preserve">555-555-1358</t>
-  </si>
-  <si>
     <t xml:space="preserve">manager</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t xml:space="preserve">nate@email.com</t>
   </si>
   <si>
-    <t xml:space="preserve">555-555-5623</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jill</t>
   </si>
   <si>
@@ -173,12 +167,6 @@
     <t xml:space="preserve">Janet</t>
   </si>
   <si>
-    <t xml:space="preserve">janet@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">555-555-9991</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clair</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bob@email.com</t>
   </si>
   <si>
     <t xml:space="preserve">555-555-4498</t>
@@ -484,10 +469,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
@@ -617,19 +602,16 @@
       <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="G5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
@@ -641,21 +623,21 @@
         <v>45000</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6</v>
@@ -667,21 +649,21 @@
         <v>150000</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>7</v>
@@ -693,10 +675,7 @@
         <v>35000</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>12</v>
@@ -707,7 +686,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>8</v>
@@ -719,21 +698,21 @@
         <v>450000</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>9</v>
@@ -745,21 +724,21 @@
         <v>12000</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10</v>
@@ -770,12 +749,7 @@
       <c r="D11" s="0" t="n">
         <v>150000</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>51</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="G11" s="0" t="s">
         <v>22</v>
       </c>
@@ -785,7 +759,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>11</v>
@@ -797,21 +771,21 @@
         <v>62000</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>12</v>
@@ -823,21 +797,21 @@
         <v>40000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>13</v>
@@ -849,21 +823,21 @@
         <v>152000</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>14</v>
@@ -875,21 +849,21 @@
         <v>300000</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>15</v>
@@ -901,21 +875,21 @@
         <v>15000</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>16</v>
@@ -926,22 +900,20 @@
       <c r="D17" s="0" t="n">
         <v>45000</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>17</v>
@@ -953,21 +925,21 @@
         <v>200000</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>18</v>
@@ -979,10 +951,10 @@
         <v>20000</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>22</v>
@@ -993,7 +965,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>19</v>
@@ -1005,21 +977,21 @@
         <v>20000</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>20</v>
@@ -1031,21 +1003,21 @@
         <v>63800</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>21</v>
@@ -1057,18 +1029,18 @@
         <v>425000</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>22</v>
@@ -1080,18 +1052,18 @@
         <v>25000</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>23</v>
@@ -1103,16 +1075,16 @@
         <v>45000</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1126,20 +1098,18 @@
     <hyperlink ref="E8" r:id="rId7" display="nate@email.com"/>
     <hyperlink ref="E9" r:id="rId8" display="jill@email.com"/>
     <hyperlink ref="E10" r:id="rId9" display="carl@email.com"/>
-    <hyperlink ref="E11" r:id="rId10" display="janet@email.com"/>
-    <hyperlink ref="E12" r:id="rId11" display="clair@email.com"/>
-    <hyperlink ref="E13" r:id="rId12" display="justin@email.com"/>
-    <hyperlink ref="E14" r:id="rId13" display="tim@email.com"/>
-    <hyperlink ref="E15" r:id="rId14" display="victor@email.com"/>
-    <hyperlink ref="E16" r:id="rId15" display="samantha@email.com"/>
-    <hyperlink ref="E17" r:id="rId16" display="bob@email.com"/>
-    <hyperlink ref="E18" r:id="rId17" display="adam@email.com"/>
-    <hyperlink ref="E19" r:id="rId18" display="denise@email.com"/>
-    <hyperlink ref="E20" r:id="rId19" display="gret@email.com"/>
-    <hyperlink ref="E21" r:id="rId20" display="lucy@email.com"/>
-    <hyperlink ref="E22" r:id="rId21" display="megan@email.com"/>
-    <hyperlink ref="E23" r:id="rId22" display="sally@email.com"/>
-    <hyperlink ref="E24" r:id="rId23" display="frank@email.com"/>
+    <hyperlink ref="E12" r:id="rId10" display="clair@email.com"/>
+    <hyperlink ref="E13" r:id="rId11" display="justin@email.com"/>
+    <hyperlink ref="E14" r:id="rId12" display="tim@email.com"/>
+    <hyperlink ref="E15" r:id="rId13" display="victor@email.com"/>
+    <hyperlink ref="E16" r:id="rId14" display="samantha@email.com"/>
+    <hyperlink ref="E18" r:id="rId15" display="adam@email.com"/>
+    <hyperlink ref="E19" r:id="rId16" display="denise@email.com"/>
+    <hyperlink ref="E20" r:id="rId17" display="gret@email.com"/>
+    <hyperlink ref="E21" r:id="rId18" display="lucy@email.com"/>
+    <hyperlink ref="E22" r:id="rId19" display="megan@email.com"/>
+    <hyperlink ref="E23" r:id="rId20" display="sally@email.com"/>
+    <hyperlink ref="E24" r:id="rId21" display="frank@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1162,65 +1132,65 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed operators and updated pdfs
</commit_message>
<xml_diff>
--- a/Lesson_04 - Simple Select Queries Pt 2/employees.xlsx
+++ b/Lesson_04 - Simple Select Queries Pt 2/employees.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
   <si>
     <t xml:space="preserve">EMPLOYEE_NAME</t>
   </si>
@@ -348,6 +348,72 @@
   </si>
   <si>
     <t xml:space="preserve">Less than or equal to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BETWEEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Between minimum and maximum values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT BETWEEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outside minimum and maximum values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is not the case that …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matches one of a list of values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not match any of a list of values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has no value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has some value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matches pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT LIKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not match pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANY/SOME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition applies to any of a list of values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition applies to every value in a list of values </t>
   </si>
 </sst>
 </file>
@@ -469,10 +535,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
@@ -1126,13 +1192,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.83"/>
   </cols>
@@ -1191,6 +1257,94 @@
       </c>
       <c r="B7" s="0" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>